<commit_message>
Tested QamDemod with BPSK and is working
</commit_message>
<xml_diff>
--- a/Xilinx/Vivado/bd/ps_regs.xlsx
+++ b/Xilinx/Vivado/bd/ps_regs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\FAU-Modem\OFDM\Xilinx\Vivado\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805AE99F-20B1-4DF2-B7F8-D40FB56D2BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C32C7D-F8F5-44F1-828E-68443FC425F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A02FE199-425C-4A4F-828F-3CFDED17A16F}"/>
   </bookViews>
@@ -313,25 +313,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,7 +648,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,39 +663,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2">
         <v>128</v>
       </c>
     </row>
@@ -722,7 +720,7 @@
       <c r="F4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="11" t="s">
         <v>25</v>
       </c>
       <c r="H4" t="s">
@@ -739,16 +737,16 @@
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="11"/>
       <c r="H5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
@@ -760,7 +758,7 @@
       <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H7" t="s">
@@ -777,11 +775,11 @@
       <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="11" t="s">
         <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -794,7 +792,7 @@
       <c r="F9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="11"/>
       <c r="H9" t="s">
         <v>51</v>
       </c>
@@ -820,7 +818,7 @@
       <c r="F11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="11" t="s">
         <v>25</v>
       </c>
       <c r="H11" t="s">
@@ -837,7 +835,7 @@
       <c r="F12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="11"/>
       <c r="H12" t="s">
         <v>54</v>
       </c>
@@ -852,7 +850,7 @@
       <c r="F13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="11"/>
       <c r="H13" t="s">
         <v>52</v>
       </c>
@@ -878,7 +876,7 @@
       <c r="F15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="11" t="s">
         <v>25</v>
       </c>
       <c r="H15" t="s">
@@ -895,7 +893,7 @@
       <c r="F16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="4"/>
+      <c r="G16" s="11"/>
       <c r="H16" t="s">
         <v>53</v>
       </c>
@@ -921,7 +919,7 @@
       <c r="F18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H18" t="s">
@@ -938,7 +936,7 @@
       <c r="F19" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">

</xml_diff>

<commit_message>
Added Synchronizer into radio top and SW
</commit_message>
<xml_diff>
--- a/Xilinx/Vivado/bd/ps_regs.xlsx
+++ b/Xilinx/Vivado/bd/ps_regs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\FAU-Modem\OFDM\Xilinx\Vivado\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C32C7D-F8F5-44F1-828E-68443FC425F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4980986C-EF66-440B-A283-D60F086AD4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A02FE199-425C-4A4F-828F-3CFDED17A16F}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="130">
   <si>
     <t>Register Name</t>
   </si>
@@ -110,9 +111,6 @@
     <t>0x0</t>
   </si>
   <si>
-    <t>Configured at Same Time</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -216,6 +214,219 @@
   </si>
   <si>
     <t>Configure FFT core on 0 to 1 transition</t>
+  </si>
+  <si>
+    <t>Version 2</t>
+  </si>
+  <si>
+    <t>Fc_scaled</t>
+  </si>
+  <si>
+    <t>[31:0]</t>
+  </si>
+  <si>
+    <t>0x00A3D70A</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>0x8</t>
+  </si>
+  <si>
+    <t>SW/HW access</t>
+  </si>
+  <si>
+    <t>decimate_ratio</t>
+  </si>
+  <si>
+    <t>0x28</t>
+  </si>
+  <si>
+    <t>rw/ro</t>
+  </si>
+  <si>
+    <t>DAC_Control</t>
+  </si>
+  <si>
+    <t>[19:16]</t>
+  </si>
+  <si>
+    <t>ADC_Control</t>
+  </si>
+  <si>
+    <t>[23:20]</t>
+  </si>
+  <si>
+    <t>ADC_Status</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>ro/wo</t>
+  </si>
+  <si>
+    <t>Interp_ratio</t>
+  </si>
+  <si>
+    <t>DMA_loopback</t>
+  </si>
+  <si>
+    <t>Symbols</t>
+  </si>
+  <si>
+    <t>[20:17]</t>
+  </si>
+  <si>
+    <t>0x1</t>
+  </si>
+  <si>
+    <t>OFDM Symbols in a pcacket</t>
+  </si>
+  <si>
+    <t>threshold</t>
+  </si>
+  <si>
+    <t>0x0002D464</t>
+  </si>
+  <si>
+    <t>Peak threshold for Synchronization</t>
+  </si>
+  <si>
+    <t>[11:0]</t>
+  </si>
+  <si>
+    <t>0x400</t>
+  </si>
+  <si>
+    <t>N point FFT</t>
+  </si>
+  <si>
+    <t>[23:12]</t>
+  </si>
+  <si>
+    <t>0x100</t>
+  </si>
+  <si>
+    <t>Cyclic Prefix</t>
+  </si>
+  <si>
+    <t>sync_loopback</t>
+  </si>
+  <si>
+    <t>[24]</t>
+  </si>
+  <si>
+    <t>Sync function DMA loopback enable</t>
+  </si>
+  <si>
+    <t>Utilization</t>
+  </si>
+  <si>
+    <t>LUT:</t>
+  </si>
+  <si>
+    <t>LUTRAM</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>BRAM</t>
+  </si>
+  <si>
+    <t>DSP</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>9271 (52.68%)</t>
+  </si>
+  <si>
+    <t>569 (9.48%)</t>
+  </si>
+  <si>
+    <t>13028 (37.01%)</t>
+  </si>
+  <si>
+    <t>17 (28.33)</t>
+  </si>
+  <si>
+    <t>37 (46.25)</t>
+  </si>
+  <si>
+    <t>Available:</t>
+  </si>
+  <si>
+    <t>1716 (9.75%)</t>
+  </si>
+  <si>
+    <t>51 (0.85%)</t>
+  </si>
+  <si>
+    <t>2266 (6.44%)</t>
+  </si>
+  <si>
+    <t>0 (0%)</t>
+  </si>
+  <si>
+    <t>PS_Zynq:</t>
+  </si>
+  <si>
+    <t>DAC_Chain:</t>
+  </si>
+  <si>
+    <t>321 (1.82%)</t>
+  </si>
+  <si>
+    <t>48 (0.8%)</t>
+  </si>
+  <si>
+    <t>673 (1.91%)</t>
+  </si>
+  <si>
+    <t>0.5 (0.83%)</t>
+  </si>
+  <si>
+    <t>4 (5%)</t>
+  </si>
+  <si>
+    <t>ADC_Chain:</t>
+  </si>
+  <si>
+    <t>346 (1.97%)</t>
+  </si>
+  <si>
+    <t>31 (0.52%)</t>
+  </si>
+  <si>
+    <t>573 (1.63%)</t>
+  </si>
+  <si>
+    <t>1 (1.67%)</t>
+  </si>
+  <si>
+    <t>5 (6.25)</t>
+  </si>
+  <si>
+    <t>Synchronizer</t>
+  </si>
+  <si>
+    <t>3564 (20.25%)</t>
+  </si>
+  <si>
+    <t>53 (0.88%)</t>
+  </si>
+  <si>
+    <t>4324 (12.3%)</t>
+  </si>
+  <si>
+    <t>11 (18.3%)</t>
+  </si>
+  <si>
+    <t>28 (35%)</t>
   </si>
 </sst>
 </file>
@@ -245,7 +456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,6 +511,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -313,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -327,9 +544,12 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,25 +864,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429789EE-5917-404B-B4D4-C27E5151BD8B}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" customWidth="1"/>
-    <col min="8" max="8" width="52.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="52.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -672,23 +894,26 @@
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -699,7 +924,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -710,94 +935,94 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="1" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" t="s">
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -808,137 +1033,137 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="1" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="F12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="11"/>
-      <c r="H13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
         <v>16</v>
       </c>
-      <c r="E14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="11"/>
-      <c r="H16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F19" t="s">
         <v>46</v>
       </c>
-      <c r="F17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -949,7 +1174,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -960,12 +1185,426 @@
         <v>13</v>
       </c>
     </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" t="s">
+        <v>72</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" t="s">
+        <v>42</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36" t="s">
+        <v>79</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" t="s">
+        <v>85</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="13">
+        <v>17600</v>
+      </c>
+      <c r="C48" s="13">
+        <v>6000</v>
+      </c>
+      <c r="D48" s="13">
+        <v>35200</v>
+      </c>
+      <c r="E48" s="13">
+        <v>60</v>
+      </c>
+      <c r="F48" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" t="s">
+        <v>104</v>
+      </c>
+      <c r="F49" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E50" t="s">
+        <v>110</v>
+      </c>
+      <c r="F50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E51" t="s">
+        <v>116</v>
+      </c>
+      <c r="F51" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" t="s">
+        <v>126</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E53" t="s">
+        <v>128</v>
+      </c>
+      <c r="F53" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H15:H16"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>